<commit_message>
The Latest results of the Arena
</commit_message>
<xml_diff>
--- a/model_arena_results.xlsx
+++ b/model_arena_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9120"/>
+    <workbookView windowWidth="23040" windowHeight="9180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,13 +53,13 @@
     <t>meta-llama/llama-3.3-70b-instruct:free</t>
   </si>
   <si>
+    <t>google/gemma-3-27b-it:free</t>
+  </si>
+  <si>
     <t>qwen/qwq-32b:free</t>
   </si>
   <si>
     <t>open-r1/olympiccoder-32b:free</t>
-  </si>
-  <si>
-    <t>google/gemma-3-27b-it:free</t>
   </si>
   <si>
     <t>cognitivecomputations/dolphin3.0-r1-mistral-24b:free</t>
@@ -775,6 +775,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:F9" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F9" etc:filterBottomFollowUsedRange="0"/>
+  <sortState ref="A2:F9">
+    <sortCondition ref="B1" descending="1"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Model"/>
+    <tableColumn id="2" name="ELO"/>
+    <tableColumn id="3" name="Average Response Time"/>
+    <tableColumn id="4" name="Average Token Size"/>
+    <tableColumn id="5" name="Total runs"/>
+    <tableColumn id="6" name="Failures"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1065,7 +1083,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="$A5:$XFD5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1095,16 +1113,16 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>2530</v>
+        <v>2336</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>4.18</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1115,16 +1133,16 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>2152</v>
+        <v>2058</v>
       </c>
       <c r="C3">
-        <v>3.12</v>
+        <v>4.41</v>
       </c>
       <c r="D3">
-        <v>22</v>
+        <v>66.5</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1135,16 +1153,16 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>1820</v>
+        <v>1959</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>20.21</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>721.75</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1155,16 +1173,16 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>1820</v>
+        <v>1836</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>19.76</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>666</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1175,16 +1193,16 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>1770</v>
+        <v>1800</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>48.77</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>167.33</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1215,16 +1233,16 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>1570</v>
+        <v>1687</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>25.14</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>204.5</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1235,16 +1253,16 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>1548</v>
+        <v>1531</v>
       </c>
       <c r="C9">
-        <v>2.46</v>
+        <v>14.76</v>
       </c>
       <c r="D9">
-        <v>20</v>
+        <v>477.2</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1253,5 +1271,8 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding the API & HTML generation
</commit_message>
<xml_diff>
--- a/model_arena_results.xlsx
+++ b/model_arena_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9180"/>
+    <workbookView windowWidth="23040" windowHeight="9120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
     <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,13 +92,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -566,148 +559,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -780,7 +773,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:F9" totalsRowShown="0">
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F9" etc:filterBottomFollowUsedRange="0"/>
-  <sortState ref="A2:F9">
+  <sortState ref="A1:F9">
     <sortCondition ref="B1" descending="1"/>
   </sortState>
   <tableColumns count="6">
@@ -1083,7 +1076,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>

</xml_diff>